<commit_message>
mise à jour quatrième semaine
</commit_message>
<xml_diff>
--- a/Gestion de projet/Matrice de traçabilité.xlsx
+++ b/Gestion de projet/Matrice de traçabilité.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="281">
   <si>
     <t>E_TAX_10</t>
   </si>
@@ -708,15 +708,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Une documentation spécifique devra être fournie pour chaque lot.
-Cette documentation sera composée, au minimum :
--          d’une spécification technique détaillée du lot,
--          d’un document de conception pour chaque composant à réaliser,
--          d’un plan de validation du lot,
--          si besoin, d’une description des interfaces (du type javadoc ou doxygen) ou d’une notice d’utilisation pour chaque composant.
-Chacun de ces documents devra être visé par la maîtrise d’œuvre du projet avant livraison à la maîtrise d’ouvrage.</t>
-  </si>
-  <si>
     <t>PDM</t>
   </si>
   <si>
@@ -746,13 +737,6 @@
 -          Une fiche de version de l’application livrée décrivant les exigences couvertes par la version de l’application, les évolutions prises en charge par la version, les limites éventuelles et les anomalies résiduelles,
 -          Un bilan de validation de la version de l’application mettant en avant les résultats de l’exécution du plan de test.
 </t>
-  </si>
-  <si>
-    <t>Chaque responsable de lot devra fournir un plan de développement comprenant à minima : 
--          Une description et la justification de l’organisation mise en place pour la conduite du développement du lot.
--          Une description des rôles et des responsabilités au sein de l’équipe de développement du lot.
--          Un planning général faisant apparaître les principales tâches réalisées dans le cadre du développement du lot.
--          Une analyse des principaux risques identifiés.</t>
   </si>
   <si>
     <t>Pour chaque jalon, le maître d'œuvre du projet «SPORTIFS» devra fournir un planning à jour présentant l'avancement des différentes tâches.</t>
@@ -780,6 +764,149 @@
   </si>
   <si>
     <t>Voir le registre des livrables</t>
+  </si>
+  <si>
+    <t>STB_COL_03, STB_COL_06</t>
+  </si>
+  <si>
+    <t>STB_COL_02</t>
+  </si>
+  <si>
+    <t>STB_COL_04</t>
+  </si>
+  <si>
+    <t>STB_EXT_01</t>
+  </si>
+  <si>
+    <t>STB_EXT_02</t>
+  </si>
+  <si>
+    <t>STB_EXT_03</t>
+  </si>
+  <si>
+    <t>STB_EXT_04</t>
+  </si>
+  <si>
+    <t>STB_EXT_05</t>
+  </si>
+  <si>
+    <t>STB_CLA_02</t>
+  </si>
+  <si>
+    <t>STB_TAX_02</t>
+  </si>
+  <si>
+    <t>STB_TAX_01</t>
+  </si>
+  <si>
+    <t>STB_TAX_04</t>
+  </si>
+  <si>
+    <t>STB_ALT_01</t>
+  </si>
+  <si>
+    <t>STB_ADM_01</t>
+  </si>
+  <si>
+    <t>STB_SUP_12</t>
+  </si>
+  <si>
+    <t>STB_SUP_04</t>
+  </si>
+  <si>
+    <t>STB_SUP_03</t>
+  </si>
+  <si>
+    <t>Jaune/Orange</t>
+  </si>
+  <si>
+    <t>STB_USER_11</t>
+  </si>
+  <si>
+    <t>STB_USER_09</t>
+  </si>
+  <si>
+    <t>STB_USER_07</t>
+  </si>
+  <si>
+    <t>STB_USER_04</t>
+  </si>
+  <si>
+    <t>STB_SEA_06, STB_USER_11</t>
+  </si>
+  <si>
+    <t>STB_TAX_03, STB_SUP_02</t>
+  </si>
+  <si>
+    <t>STB_COL_01, STB_USER_12</t>
+  </si>
+  <si>
+    <t>STB_SUP_07, STB_SUP_06, STB_SUP_08</t>
+  </si>
+  <si>
+    <t>STB_COL_05, STB_SUP_08</t>
+  </si>
+  <si>
+    <t>STB_CLA_03, STB_SUP_04</t>
+  </si>
+  <si>
+    <t>STB_CLA_04, STB_CLA_05, STB_SUP_05</t>
+  </si>
+  <si>
+    <t>STB_CLA_07, STB_SUP_04</t>
+  </si>
+  <si>
+    <t>STB_CLA_08, STB_SUP_10</t>
+  </si>
+  <si>
+    <t>STB_CLA_06, STB_SUP_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STB_IND_01, STB_IND_02, STB_IND_03, STB_IND_04, STB_IND_06, STB_IND_07
+</t>
+  </si>
+  <si>
+    <t>STB_SEA_01, STB_USER_01</t>
+  </si>
+  <si>
+    <t>STB_SEA_03, STB_USER_08</t>
+  </si>
+  <si>
+    <t>STB_SEA_04, STB_USER_11</t>
+  </si>
+  <si>
+    <t>STB_SEA_02, STB_USER_11</t>
+  </si>
+  <si>
+    <t>STB_SEA_05, STB_IND_05, STB_USER_02</t>
+  </si>
+  <si>
+    <t>STB_USER_10, STB_USER_03</t>
+  </si>
+  <si>
+    <t>STB_SUP_01, STB_USER_06</t>
+  </si>
+  <si>
+    <t>STB_SUP_12, STB_USER_05</t>
+  </si>
+  <si>
+    <t>STB_LOG_01, STB_ADM_02</t>
+  </si>
+  <si>
+    <t>Chaque responsable de lot devra fournir un plan de développement comprenant à minima : 
+- Une description et la justification de l’organisation mise en place pour la conduite du développement du lot.
+- Une description des rôles et des responsabilités au sein de l’équipe de développement du lot.
+- Un planning général faisant apparaître les principales tâches réalisées dans le cadre du développement du lot.
+- Une analyse des principaux risques identifiés.</t>
+  </si>
+  <si>
+    <t>Une documentation spécifique devra être fournie pour chaque lot.
+Cette documentation sera composée, au minimum :
+- d’une spécification technique détaillée du lot,
+- d’un document de conception pour chaque composant à réaliser,
+- d’un plan de validation du lot,
+- si besoin, d’une description des interfaces (du type javadoc ou doxygen) ou d’une notice d’utilisation pour chaque composant.
+Chacun de ces documents devra être visé par la maîtrise d’œuvre du projet avant livraison à la maîtrise d’ouvrage.</t>
   </si>
 </sst>
 </file>
@@ -894,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -940,6 +1067,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1294,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1048544"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>220</v>
@@ -1351,7 +1481,9 @@
       <c r="F2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1361,7 +1493,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>220</v>
@@ -1382,7 +1514,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>220</v>
@@ -1403,7 +1535,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>220</v>
@@ -1414,7 +1546,9 @@
       <c r="F5" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1424,7 +1558,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>220</v>
@@ -1435,7 +1569,9 @@
       <c r="F6" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1445,7 +1581,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>220</v>
@@ -1456,7 +1592,9 @@
       <c r="F7" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1466,16 +1604,20 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1485,7 +1627,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>220</v>
@@ -1506,7 +1648,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>220</v>
@@ -1517,7 +1659,9 @@
       <c r="F10" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1527,7 +1671,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>220</v>
@@ -1536,9 +1680,11 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G11" s="2"/>
+        <v>254</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1548,7 +1694,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>220</v>
@@ -1582,7 +1728,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>220</v>
@@ -1591,7 +1737,9 @@
       <c r="F14" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1601,7 +1749,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>220</v>
@@ -1612,7 +1760,9 @@
       <c r="F15" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1622,16 +1772,20 @@
         <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8">
+        <v>2</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1641,7 +1795,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>220</v>
@@ -1652,7 +1806,9 @@
       <c r="F17" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1662,7 +1818,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>220</v>
@@ -1673,7 +1829,9 @@
       <c r="F18" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1683,7 +1841,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>220</v>
@@ -1694,7 +1852,9 @@
       <c r="F19" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1704,7 +1864,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>220</v>
@@ -1723,7 +1883,7 @@
         <v>209</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>220</v>
@@ -1734,7 +1894,9 @@
       <c r="F21" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1744,7 +1906,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>220</v>
@@ -1763,7 +1925,7 @@
         <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D23" s="16" t="s">
         <v>220</v>
@@ -1790,52 +1952,54 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="E25" s="32">
+      <c r="C25" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" s="33">
         <v>1</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="G25" s="22"/>
+      <c r="G25" s="26" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="23"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="23"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="24"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1845,7 +2009,7 @@
         <v>47</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>220</v>
@@ -1856,7 +2020,9 @@
       <c r="F29" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -1881,7 +2047,7 @@
         <v>51</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>220</v>
@@ -1892,7 +2058,9 @@
       <c r="F31" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1902,7 +2070,7 @@
         <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>220</v>
@@ -1921,7 +2089,7 @@
         <v>55</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>220</v>
@@ -1930,7 +2098,9 @@
       <c r="F33" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G33" s="2"/>
+      <c r="G33" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1940,7 +2110,7 @@
         <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>220</v>
@@ -1949,7 +2119,9 @@
       <c r="F34" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -1959,7 +2131,7 @@
         <v>59</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>220</v>
@@ -1980,7 +2152,7 @@
         <v>61</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>220</v>
@@ -1989,7 +2161,9 @@
       <c r="F36" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
@@ -1999,7 +2173,7 @@
         <v>63</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>220</v>
@@ -2018,7 +2192,7 @@
         <v>65</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>220</v>
@@ -2027,7 +2201,9 @@
       <c r="F38" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -2037,7 +2213,7 @@
         <v>67</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>220</v>
@@ -2048,7 +2224,9 @@
       <c r="F39" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -2058,7 +2236,7 @@
         <v>69</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>220</v>
@@ -2069,7 +2247,9 @@
       <c r="F40" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -2079,7 +2259,7 @@
         <v>71</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>220</v>
@@ -2090,7 +2270,9 @@
       <c r="F41" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -2100,7 +2282,7 @@
         <v>73</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>220</v>
@@ -2111,7 +2293,9 @@
       <c r="F42" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -2121,7 +2305,7 @@
         <v>75</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>220</v>
@@ -2132,7 +2316,7 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>76</v>
       </c>
@@ -2140,7 +2324,7 @@
         <v>77</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>220</v>
@@ -2151,117 +2335,123 @@
       <c r="F44" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G44" s="2"/>
+      <c r="G44" s="19" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="C45" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="22" t="s">
+      <c r="C45" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E45" s="33"/>
+      <c r="F45" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="G45" s="22"/>
+      <c r="G45" s="23" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="E50" s="28"/>
-      <c r="F50" s="22" t="s">
+      <c r="C50" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E50" s="29"/>
+      <c r="F50" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="G50" s="22"/>
+      <c r="G50" s="23" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
+      <c r="A51" s="32"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="31"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
+      <c r="A53" s="32"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="31"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
     </row>
     <row r="55" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -2271,7 +2461,7 @@
         <v>81</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>220</v>
@@ -2280,7 +2470,9 @@
       <c r="F55" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G55" s="2"/>
+      <c r="G55" s="2" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
@@ -2290,7 +2482,7 @@
         <v>83</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>220</v>
@@ -2299,7 +2491,9 @@
       <c r="F56" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G56" s="2"/>
+      <c r="G56" s="2" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2309,7 +2503,7 @@
         <v>85</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>220</v>
@@ -2318,7 +2512,9 @@
       <c r="F57" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G57" s="2"/>
+      <c r="G57" s="2" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="48" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -2328,7 +2524,7 @@
         <v>87</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>220</v>
@@ -2337,7 +2533,9 @@
       <c r="F58" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G58" s="2"/>
+      <c r="G58" s="2" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="59" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -2347,7 +2545,7 @@
         <v>89</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>220</v>
@@ -2356,7 +2554,9 @@
       <c r="F59" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G59" s="2"/>
+      <c r="G59" s="2" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
@@ -2366,7 +2566,7 @@
         <v>91</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>220</v>
@@ -2375,7 +2575,9 @@
       <c r="F60" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G60" s="2"/>
+      <c r="G60" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="61" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -2385,7 +2587,7 @@
         <v>93</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>220</v>
@@ -2394,7 +2596,9 @@
       <c r="F61" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G61" s="2"/>
+      <c r="G61" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
@@ -2404,7 +2608,7 @@
         <v>95</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>220</v>
@@ -2413,7 +2617,9 @@
       <c r="F62" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G62" s="2"/>
+      <c r="G62" s="2" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="63" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -2423,7 +2629,7 @@
         <v>97</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>220</v>
@@ -2432,7 +2638,9 @@
       <c r="F63" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G63" s="2"/>
+      <c r="G63" s="2" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -2442,7 +2650,7 @@
         <v>99</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>220</v>
@@ -2461,7 +2669,7 @@
         <v>101</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>220</v>
@@ -2470,7 +2678,9 @@
       <c r="F65" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G65" s="2"/>
+      <c r="G65" s="2" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="66" spans="1:7" ht="48" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
@@ -2480,7 +2690,7 @@
         <v>103</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>220</v>
@@ -2499,7 +2709,7 @@
         <v>105</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>220</v>
@@ -2508,7 +2718,9 @@
       <c r="F67" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G67" s="2"/>
+      <c r="G67" s="2" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -2518,7 +2730,7 @@
         <v>107</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>220</v>
@@ -2527,7 +2739,9 @@
       <c r="F68" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G68" s="2"/>
+      <c r="G68" s="2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="69" spans="1:7" ht="48" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
@@ -2537,7 +2751,7 @@
         <v>109</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>220</v>
@@ -2546,7 +2760,9 @@
       <c r="F69" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G69" s="2"/>
+      <c r="G69" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="70" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -2556,7 +2772,7 @@
         <v>111</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>220</v>
@@ -2565,7 +2781,9 @@
       <c r="F70" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G70" s="2"/>
+      <c r="G70" s="2" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="71" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
@@ -2575,7 +2793,7 @@
         <v>113</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>220</v>
@@ -2584,7 +2802,9 @@
       <c r="F71" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G71" s="2"/>
+      <c r="G71" s="2" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="72" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
@@ -2594,7 +2814,7 @@
         <v>115</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>220</v>
@@ -2603,7 +2823,9 @@
       <c r="F72" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G72" s="2"/>
+      <c r="G72" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="73" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
@@ -2613,7 +2835,7 @@
         <v>117</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>220</v>
@@ -2622,7 +2844,9 @@
       <c r="F73" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G73" s="2"/>
+      <c r="G73" s="2" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="74" spans="1:7" ht="72" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
@@ -2632,7 +2856,7 @@
         <v>119</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>219</v>
@@ -2651,7 +2875,7 @@
         <v>121</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>219</v>
@@ -2670,7 +2894,7 @@
         <v>123</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>219</v>
@@ -2689,7 +2913,7 @@
         <v>125</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>219</v>
@@ -2708,7 +2932,7 @@
         <v>127</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>219</v>
@@ -2727,7 +2951,7 @@
         <v>129</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>220</v>
@@ -2746,7 +2970,7 @@
         <v>131</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>220</v>
@@ -2765,7 +2989,7 @@
         <v>133</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>220</v>
@@ -2784,7 +3008,7 @@
         <v>135</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>220</v>
@@ -2803,7 +3027,7 @@
         <v>137</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>220</v>
@@ -2822,7 +3046,7 @@
         <v>139</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>220</v>
@@ -2841,7 +3065,7 @@
         <v>141</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>220</v>
@@ -2860,7 +3084,7 @@
         <v>217</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>221</v>
@@ -2876,10 +3100,10 @@
         <v>143</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>220</v>
@@ -2898,7 +3122,7 @@
         <v>145</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>221</v>
@@ -2917,7 +3141,7 @@
         <v>147</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>221</v>
@@ -2936,7 +3160,7 @@
         <v>149</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>220</v>
@@ -2955,7 +3179,7 @@
         <v>151</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>219</v>
@@ -2971,10 +3195,10 @@
         <v>152</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>221</v>
@@ -2990,10 +3214,10 @@
         <v>153</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>221</v>
@@ -3012,7 +3236,7 @@
         <v>155</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>221</v>
@@ -3031,7 +3255,7 @@
         <v>157</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>221</v>
@@ -3050,7 +3274,7 @@
         <v>159</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>221</v>
@@ -3066,10 +3290,10 @@
         <v>160</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>219</v>
@@ -3088,7 +3312,7 @@
         <v>162</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>219</v>
@@ -3104,10 +3328,10 @@
         <v>163</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>221</v>
@@ -3126,7 +3350,7 @@
         <v>165</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>221</v>
@@ -3145,7 +3369,7 @@
         <v>167</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>221</v>
@@ -3161,10 +3385,10 @@
         <v>168</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>219</v>
@@ -3183,10 +3407,10 @@
         <v>170</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="2" t="s">
@@ -3202,7 +3426,7 @@
         <v>172</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>219</v>
@@ -3221,7 +3445,7 @@
         <v>174</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>219</v>
@@ -3240,7 +3464,7 @@
         <v>176</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>219</v>
@@ -3250,7 +3474,7 @@
         <v>216</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="156" x14ac:dyDescent="0.25">
@@ -3258,10 +3482,10 @@
         <v>177</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>220</v>
@@ -3277,10 +3501,10 @@
         <v>178</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>221</v>
@@ -3299,7 +3523,7 @@
         <v>180</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>220</v>
@@ -3318,7 +3542,7 @@
         <v>182</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>220</v>
@@ -3337,7 +3561,7 @@
         <v>184</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>220</v>
@@ -3356,7 +3580,7 @@
         <v>186</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>220</v>
@@ -3375,7 +3599,7 @@
         <v>188</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>219</v>
@@ -3394,7 +3618,7 @@
         <v>190</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>220</v>
@@ -3413,7 +3637,7 @@
         <v>192</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>220</v>
@@ -3426,7 +3650,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D119">
         <f>COUNTIF(D2:D115,"PC")</f>
@@ -3435,7 +3659,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D120">
         <f>COUNTIF(D2:D115,"PS")</f>
@@ -3444,7 +3668,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B121" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D121">
         <f>COUNTIF(D2:D115,"S")</f>
@@ -3453,7 +3677,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D122">
         <f>COUNTIF(D2:D115,"V")</f>

</xml_diff>